<commit_message>
corrigida importacao de planilha para evitar gasto excessivo de memoria
</commit_message>
<xml_diff>
--- a/application/uploads/vendas/planilha.xlsx
+++ b/application/uploads/vendas/planilha.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="56">
   <si>
     <t xml:space="preserve">CNPJ</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t xml:space="preserve">88120-003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">becomex3</t>
   </si>
   <si>
     <t xml:space="preserve">Teste</t>
@@ -472,19 +469,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,6 +494,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,6 +510,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,27 +526,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,91 +554,91 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="19" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="19" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="20" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="20" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -641,7 +646,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="24" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="24" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -653,12 +658,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Campo da tabela dinâmica" xfId="20"/>
-    <cellStyle name="Canto da tabela dinâmica" xfId="21"/>
-    <cellStyle name="Categoria da tabela dinâmica" xfId="22"/>
-    <cellStyle name="Resultado da tabela dinâmica" xfId="23"/>
+    <cellStyle name="Canto da tabela dinâmica" xfId="20"/>
+    <cellStyle name="Valor da tabela dinâmica" xfId="21"/>
+    <cellStyle name="Campo da tabela dinâmica" xfId="22"/>
+    <cellStyle name="Categoria da tabela dinâmica" xfId="23"/>
     <cellStyle name="Título da tabela dinâmica" xfId="24"/>
-    <cellStyle name="Valor da tabela dinâmica" xfId="25"/>
+    <cellStyle name="Resultado da tabela dinâmica" xfId="25"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -723,7 +728,599 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Soma de Valor Faturado</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Painel_Venda_Serviço!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472c4"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472c4"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffc000"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Painel_Venda_Serviço!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Descrição do Serviço</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ABC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KTM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>xyz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Painel_Venda_Serviço!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>585.294117647059</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>719.166666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Painel_Venda_Serviço!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ed7d31"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472c4"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffc000"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Painel_Venda_Serviço!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Descrição do Serviço</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ABC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KTM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>xyz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Painel_Venda_Serviço!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>108900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1039,598 +1636,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Soma de Valor Faturado</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="30"/>
-      <c:rotY val="0"/>
-      <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
-    </c:view3D>
-    <c:floor>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:backWall>
-    <c:plotArea>
-      <c:pie3DChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Painel_Venda_Serviço!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Dados</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472c4"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="a5a5a5"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffc000"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Painel_Venda_Serviço!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Descrição do Serviço</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ABC</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>KTM</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>xyz</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Painel_Venda_Serviço!$B$4:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="1">
-                  <c:v>934.999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>585.294117647059</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>719.166666666666</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Painel_Venda_Serviço!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ed7d31"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472c4"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="a5a5a5"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffc000"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Painel_Venda_Serviço!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Descrição do Serviço</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ABC</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>KTM</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>xyz</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Painel_Venda_Serviço!$C$4:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="1">
-                  <c:v>108900</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>88000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85250</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-      </c:pie3DChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1642,9 +1647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>304560</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1652,8 +1657,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3420000" y="331560"/>
-        <a:ext cx="4593600" cy="2742480"/>
+        <a:off x="3418920" y="329760"/>
+        <a:ext cx="4589640" cy="2714040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1677,9 +1682,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>570960</xdr:colOff>
+      <xdr:colOff>571320</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1687,8 +1692,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4649400" y="285840"/>
-        <a:ext cx="4593600" cy="2742480"/>
+        <a:off x="4649040" y="284040"/>
+        <a:ext cx="4589280" cy="2714040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2355,13 +2360,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.22"/>
@@ -2371,51 +2376,51 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="16.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2438,7 +2443,7 @@
       <c r="F2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="8" t="n">
         <v>44348</v>
       </c>
       <c r="H2" s="2" t="n">
@@ -2447,17 +2452,17 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="J2" s="9" t="n">
         <f aca="false">K2/150</f>
         <v>100</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="10" t="n">
         <v>15000</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="L2" s="10" t="n">
         <v>8000</v>
       </c>
-      <c r="M2" s="8" t="n">
+      <c r="M2" s="10" t="n">
         <f aca="false">K2-L2</f>
         <v>7000</v>
       </c>
@@ -2481,7 +2486,7 @@
       <c r="F3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="8" t="n">
         <v>44349</v>
       </c>
       <c r="H3" s="2" t="n">
@@ -2490,17 +2495,17 @@
       <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="7" t="n">
+      <c r="J3" s="9" t="n">
         <f aca="false">K3/150</f>
         <v>53.3333333333333</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="10" t="n">
         <v>8000</v>
       </c>
-      <c r="L3" s="8" t="n">
+      <c r="L3" s="10" t="n">
         <v>6500</v>
       </c>
-      <c r="M3" s="8" t="n">
+      <c r="M3" s="10" t="n">
         <f aca="false">K3-L3</f>
         <v>1500</v>
       </c>
@@ -2524,7 +2529,7 @@
       <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="8" t="n">
         <v>44354</v>
       </c>
       <c r="H4" s="2" t="n">
@@ -2533,17 +2538,17 @@
       <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="7" t="n">
+      <c r="J4" s="9" t="n">
         <f aca="false">K4/150</f>
         <v>50</v>
       </c>
-      <c r="K4" s="8" t="n">
+      <c r="K4" s="10" t="n">
         <v>7500</v>
       </c>
-      <c r="L4" s="8" t="n">
+      <c r="L4" s="10" t="n">
         <v>6000</v>
       </c>
-      <c r="M4" s="8" t="n">
+      <c r="M4" s="10" t="n">
         <f aca="false">K4-L4</f>
         <v>1500</v>
       </c>
@@ -2567,7 +2572,7 @@
       <c r="F5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="8" t="n">
         <v>44357</v>
       </c>
       <c r="H5" s="2" t="n">
@@ -2576,17 +2581,17 @@
       <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="9" t="n">
         <f aca="false">K5/150</f>
         <v>80</v>
       </c>
-      <c r="K5" s="8" t="n">
+      <c r="K5" s="10" t="n">
         <v>12000</v>
       </c>
-      <c r="L5" s="8" t="n">
+      <c r="L5" s="10" t="n">
         <v>8000</v>
       </c>
-      <c r="M5" s="8" t="n">
+      <c r="M5" s="10" t="n">
         <f aca="false">K5-L5</f>
         <v>4000</v>
       </c>
@@ -2610,7 +2615,7 @@
       <c r="F6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="8" t="n">
         <v>44361</v>
       </c>
       <c r="H6" s="2" t="n">
@@ -2619,17 +2624,17 @@
       <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="7" t="n">
+      <c r="J6" s="9" t="n">
         <f aca="false">K6/150</f>
         <v>36</v>
       </c>
-      <c r="K6" s="8" t="n">
+      <c r="K6" s="10" t="n">
         <v>5400</v>
       </c>
-      <c r="L6" s="8" t="n">
+      <c r="L6" s="10" t="n">
         <v>5000</v>
       </c>
-      <c r="M6" s="8" t="n">
+      <c r="M6" s="10" t="n">
         <f aca="false">K6-L6</f>
         <v>400</v>
       </c>
@@ -2653,7 +2658,7 @@
       <c r="F7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="8" t="n">
         <v>44362</v>
       </c>
       <c r="H7" s="2" t="n">
@@ -2662,17 +2667,17 @@
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="7" t="n">
+      <c r="J7" s="9" t="n">
         <f aca="false">K7/150</f>
         <v>9</v>
       </c>
-      <c r="K7" s="8" t="n">
+      <c r="K7" s="10" t="n">
         <v>1350</v>
       </c>
-      <c r="L7" s="8" t="n">
+      <c r="L7" s="10" t="n">
         <v>1400</v>
       </c>
-      <c r="M7" s="8" t="n">
+      <c r="M7" s="10" t="n">
         <f aca="false">K7-L7</f>
         <v>-50</v>
       </c>
@@ -2696,7 +2701,7 @@
       <c r="F8" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="8" t="n">
         <v>44349</v>
       </c>
       <c r="H8" s="2" t="n">
@@ -2705,17 +2710,17 @@
       <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="9" t="n">
         <f aca="false">K8/150</f>
         <v>333.333333333333</v>
       </c>
-      <c r="K8" s="8" t="n">
+      <c r="K8" s="10" t="n">
         <v>50000</v>
       </c>
-      <c r="L8" s="8" t="n">
+      <c r="L8" s="10" t="n">
         <v>45000</v>
       </c>
-      <c r="M8" s="8" t="n">
+      <c r="M8" s="10" t="n">
         <f aca="false">K8-L8</f>
         <v>5000</v>
       </c>
@@ -2739,7 +2744,7 @@
       <c r="F9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="8" t="n">
         <v>44362</v>
       </c>
       <c r="H9" s="2" t="n">
@@ -2748,17 +2753,17 @@
       <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="7" t="n">
+      <c r="J9" s="9" t="n">
         <f aca="false">K9/150</f>
         <v>273.333333333333</v>
       </c>
-      <c r="K9" s="8" t="n">
+      <c r="K9" s="10" t="n">
         <v>41000</v>
       </c>
-      <c r="L9" s="8" t="n">
+      <c r="L9" s="10" t="n">
         <v>29000</v>
       </c>
-      <c r="M9" s="8" t="n">
+      <c r="M9" s="10" t="n">
         <f aca="false">K9-L9</f>
         <v>12000</v>
       </c>
@@ -2782,7 +2787,7 @@
       <c r="F10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="8" t="n">
         <v>44350</v>
       </c>
       <c r="H10" s="2" t="n">
@@ -2791,17 +2796,17 @@
       <c r="I10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="7" t="n">
+      <c r="J10" s="9" t="n">
         <f aca="false">K10/120</f>
         <v>41.6666666666667</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="10" t="n">
         <v>5000</v>
       </c>
-      <c r="L10" s="8" t="n">
+      <c r="L10" s="10" t="n">
         <v>6500</v>
       </c>
-      <c r="M10" s="8" t="n">
+      <c r="M10" s="10" t="n">
         <f aca="false">K10-L10</f>
         <v>-1500</v>
       </c>
@@ -2825,7 +2830,7 @@
       <c r="F11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="8" t="n">
         <v>44351</v>
       </c>
       <c r="H11" s="2" t="n">
@@ -2834,17 +2839,17 @@
       <c r="I11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="7" t="n">
+      <c r="J11" s="9" t="n">
         <f aca="false">K11/120</f>
         <v>29.1666666666667</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="10" t="n">
         <v>3500</v>
       </c>
-      <c r="L11" s="8" t="n">
+      <c r="L11" s="10" t="n">
         <v>1600</v>
       </c>
-      <c r="M11" s="8" t="n">
+      <c r="M11" s="10" t="n">
         <f aca="false">K11-L11</f>
         <v>1900</v>
       </c>
@@ -2868,7 +2873,7 @@
       <c r="F12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="6" t="n">
+      <c r="G12" s="8" t="n">
         <v>44353</v>
       </c>
       <c r="H12" s="2" t="n">
@@ -2877,17 +2882,17 @@
       <c r="I12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="7" t="n">
+      <c r="J12" s="9" t="n">
         <f aca="false">K12/120</f>
         <v>63.3333333333333</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="10" t="n">
         <v>7600</v>
       </c>
-      <c r="L12" s="8" t="n">
+      <c r="L12" s="10" t="n">
         <v>7000</v>
       </c>
-      <c r="M12" s="8" t="n">
+      <c r="M12" s="10" t="n">
         <f aca="false">K12-L12</f>
         <v>600</v>
       </c>
@@ -2911,7 +2916,7 @@
       <c r="F13" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="6" t="n">
+      <c r="G13" s="8" t="n">
         <v>44356</v>
       </c>
       <c r="H13" s="2" t="n">
@@ -2920,17 +2925,17 @@
       <c r="I13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="9" t="n">
         <f aca="false">K13/120</f>
         <v>10</v>
       </c>
-      <c r="K13" s="8" t="n">
+      <c r="K13" s="10" t="n">
         <v>1200</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="10" t="n">
         <v>5000</v>
       </c>
-      <c r="M13" s="8" t="n">
+      <c r="M13" s="10" t="n">
         <f aca="false">K13-L13</f>
         <v>-3800</v>
       </c>
@@ -2954,7 +2959,7 @@
       <c r="F14" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="6" t="n">
+      <c r="G14" s="8" t="n">
         <v>44359</v>
       </c>
       <c r="H14" s="2" t="n">
@@ -2963,17 +2968,17 @@
       <c r="I14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">K14/120</f>
         <v>83.3333333333333</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="10" t="n">
         <v>10000</v>
       </c>
-      <c r="L14" s="8" t="n">
+      <c r="L14" s="10" t="n">
         <v>7500</v>
       </c>
-      <c r="M14" s="8" t="n">
+      <c r="M14" s="10" t="n">
         <f aca="false">K14-L14</f>
         <v>2500</v>
       </c>
@@ -2997,7 +3002,7 @@
       <c r="F15" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="6" t="n">
+      <c r="G15" s="8" t="n">
         <v>44360</v>
       </c>
       <c r="H15" s="2" t="n">
@@ -3006,17 +3011,17 @@
       <c r="I15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">K15/120</f>
         <v>8.33333333333333</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="10" t="n">
         <v>1000</v>
       </c>
-      <c r="L15" s="8" t="n">
+      <c r="L15" s="10" t="n">
         <v>650</v>
       </c>
-      <c r="M15" s="8" t="n">
+      <c r="M15" s="10" t="n">
         <f aca="false">K15-L15</f>
         <v>350</v>
       </c>
@@ -3040,7 +3045,7 @@
       <c r="F16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="6" t="n">
+      <c r="G16" s="8" t="n">
         <v>44361</v>
       </c>
       <c r="H16" s="2" t="n">
@@ -3049,17 +3054,17 @@
       <c r="I16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="7" t="n">
+      <c r="J16" s="9" t="n">
         <f aca="false">K16/120</f>
         <v>233.333333333333</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="10" t="n">
         <v>28000</v>
       </c>
-      <c r="L16" s="8" t="n">
+      <c r="L16" s="10" t="n">
         <v>27000</v>
       </c>
-      <c r="M16" s="8" t="n">
+      <c r="M16" s="10" t="n">
         <f aca="false">K16-L16</f>
         <v>1000</v>
       </c>
@@ -3083,7 +3088,7 @@
       <c r="F17" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="6" t="n">
+      <c r="G17" s="8" t="n">
         <v>44363</v>
       </c>
       <c r="H17" s="2" t="n">
@@ -3092,17 +3097,17 @@
       <c r="I17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="7" t="n">
+      <c r="J17" s="9" t="n">
         <f aca="false">K17/120</f>
         <v>250</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="10" t="n">
         <v>30000</v>
       </c>
-      <c r="L17" s="8" t="n">
+      <c r="L17" s="10" t="n">
         <v>30000</v>
       </c>
-      <c r="M17" s="8" t="n">
+      <c r="M17" s="10" t="n">
         <f aca="false">K17-L17</f>
         <v>0</v>
       </c>
@@ -3126,7 +3131,7 @@
       <c r="F18" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="6" t="n">
+      <c r="G18" s="8" t="n">
         <v>44352</v>
       </c>
       <c r="H18" s="2" t="n">
@@ -3135,17 +3140,17 @@
       <c r="I18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="7" t="n">
+      <c r="J18" s="9" t="n">
         <f aca="false">K18/170</f>
         <v>14.7058823529412</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="10" t="n">
         <v>2500</v>
       </c>
-      <c r="L18" s="8" t="n">
+      <c r="L18" s="10" t="n">
         <v>3000</v>
       </c>
-      <c r="M18" s="8" t="n">
+      <c r="M18" s="10" t="n">
         <f aca="false">K18-L18</f>
         <v>-500</v>
       </c>
@@ -3169,7 +3174,7 @@
       <c r="F19" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="6" t="n">
+      <c r="G19" s="8" t="n">
         <v>44355</v>
       </c>
       <c r="H19" s="2" t="n">
@@ -3178,17 +3183,17 @@
       <c r="I19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="7" t="n">
+      <c r="J19" s="9" t="n">
         <f aca="false">K19/170</f>
         <v>35.2941176470588</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="10" t="n">
         <v>6000</v>
       </c>
-      <c r="L19" s="8" t="n">
+      <c r="L19" s="10" t="n">
         <v>500</v>
       </c>
-      <c r="M19" s="8" t="n">
+      <c r="M19" s="10" t="n">
         <f aca="false">K19-L19</f>
         <v>5500</v>
       </c>
@@ -3212,7 +3217,7 @@
       <c r="F20" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="6" t="n">
+      <c r="G20" s="8" t="n">
         <v>44358</v>
       </c>
       <c r="H20" s="2" t="n">
@@ -3221,17 +3226,17 @@
       <c r="I20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="7" t="n">
+      <c r="J20" s="9" t="n">
         <f aca="false">K20/170</f>
         <v>64.7058823529412</v>
       </c>
-      <c r="K20" s="8" t="n">
+      <c r="K20" s="10" t="n">
         <v>11000</v>
       </c>
-      <c r="L20" s="8" t="n">
+      <c r="L20" s="10" t="n">
         <v>8000</v>
       </c>
-      <c r="M20" s="8" t="n">
+      <c r="M20" s="10" t="n">
         <f aca="false">K20-L20</f>
         <v>3000</v>
       </c>
@@ -3255,7 +3260,7 @@
       <c r="F21" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="6" t="n">
+      <c r="G21" s="8" t="n">
         <v>44352</v>
       </c>
       <c r="H21" s="2" t="n">
@@ -3264,17 +3269,17 @@
       <c r="I21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="7" t="n">
+      <c r="J21" s="9" t="n">
         <f aca="false">K21/170</f>
         <v>188.235294117647</v>
       </c>
-      <c r="K21" s="8" t="n">
+      <c r="K21" s="10" t="n">
         <v>32000</v>
       </c>
-      <c r="L21" s="8" t="n">
+      <c r="L21" s="10" t="n">
         <v>30000</v>
       </c>
-      <c r="M21" s="8" t="n">
+      <c r="M21" s="10" t="n">
         <f aca="false">K21-L21</f>
         <v>2000</v>
       </c>
@@ -3298,7 +3303,7 @@
       <c r="F22" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="6" t="n">
+      <c r="G22" s="8" t="n">
         <v>44357</v>
       </c>
       <c r="H22" s="2" t="n">
@@ -3307,17 +3312,17 @@
       <c r="I22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J22" s="7" t="n">
+      <c r="J22" s="9" t="n">
         <f aca="false">K22/170</f>
         <v>135.294117647059</v>
       </c>
-      <c r="K22" s="8" t="n">
+      <c r="K22" s="10" t="n">
         <v>23000</v>
       </c>
-      <c r="L22" s="8" t="n">
+      <c r="L22" s="10" t="n">
         <v>24000</v>
       </c>
-      <c r="M22" s="8" t="n">
+      <c r="M22" s="10" t="n">
         <f aca="false">K22-L22</f>
         <v>-1000</v>
       </c>
@@ -3341,7 +3346,7 @@
       <c r="F23" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="6" t="n">
+      <c r="G23" s="8" t="n">
         <v>44359</v>
       </c>
       <c r="H23" s="2" t="n">
@@ -3350,17 +3355,17 @@
       <c r="I23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="7" t="n">
+      <c r="J23" s="9" t="n">
         <f aca="false">K23/170</f>
         <v>147.058823529412</v>
       </c>
-      <c r="K23" s="8" t="n">
+      <c r="K23" s="10" t="n">
         <v>25000</v>
       </c>
-      <c r="L23" s="8" t="n">
+      <c r="L23" s="10" t="n">
         <v>22500</v>
       </c>
-      <c r="M23" s="8" t="n">
+      <c r="M23" s="10" t="n">
         <f aca="false">K23-L23</f>
         <v>2500</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -3384,49 +3389,49 @@
       <c r="F24" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="6" t="n">
+      <c r="G24" s="8" t="n">
         <v>44359</v>
       </c>
       <c r="H24" s="2" t="n">
         <v>99</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J24" s="7" t="n">
+        <v>41</v>
+      </c>
+      <c r="J24" s="9" t="n">
         <v>99</v>
       </c>
-      <c r="K24" s="8" t="n">
+      <c r="K24" s="10" t="n">
         <v>99999</v>
       </c>
-      <c r="L24" s="8" t="n">
+      <c r="L24" s="10" t="n">
         <v>88888</v>
       </c>
-      <c r="M24" s="8" t="n">
+      <c r="M24" s="10" t="n">
         <f aca="false">K24-L24</f>
         <v>11111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="6" t="n">
+      <c r="G25" s="8" t="n">
         <v>44357</v>
       </c>
       <c r="H25" s="2" t="n">
@@ -3435,27 +3440,46 @@
       <c r="I25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="J25" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="K25" s="8" t="n">
+      <c r="K25" s="10" t="n">
         <v>15000</v>
       </c>
-      <c r="L25" s="8" t="n">
+      <c r="L25" s="10" t="n">
         <v>7000</v>
       </c>
-      <c r="M25" s="8" t="n">
+      <c r="M25" s="10" t="n">
         <f aca="false">K25-L25</f>
         <v>8000</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="D27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3472,63 +3496,63 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A1:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.78"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="8" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="10" t="n">
         <v>120</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="10" t="n">
         <v>170</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3545,48 +3569,48 @@
   <dimension ref="A3:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
+      <selection pane="topLeft" activeCell="N23" activeCellId="1" sqref="A1:M25 N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="14" t="n">
+        <v>678.872549019608</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="16" t="n">
+        <v>1560.58823529412</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="12" t="n">
-        <v>678.872549019608</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="14" t="n">
-        <v>1560.58823529412</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="16" t="n">
+      <c r="B6" s="18" t="n">
         <v>2239.46078431372</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="0" t="n">
         <v>1837</v>
       </c>
@@ -3594,7 +3618,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L24" s="0" t="n">
         <v>1080</v>
       </c>
@@ -3605,7 +3629,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3623,81 +3647,81 @@
   <dimension ref="A3:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A1:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.34"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="21" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25" t="n">
+        <v>935</v>
+      </c>
+      <c r="C5" s="26" t="n">
+        <v>108900</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="27" t="n">
+        <v>585.294117647059</v>
+      </c>
+      <c r="C6" s="28" t="n">
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="29" t="n">
+        <v>719.166666666667</v>
+      </c>
+      <c r="C7" s="30" t="n">
+        <v>85250</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="23" t="n">
-        <v>934.999999999999</v>
-      </c>
-      <c r="C5" s="24" t="n">
-        <v>108900</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="25" t="n">
-        <v>585.294117647059</v>
-      </c>
-      <c r="C6" s="26" t="n">
-        <v>88000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="27" t="n">
-        <v>719.166666666666</v>
-      </c>
-      <c r="C7" s="28" t="n">
-        <v>85250</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="29" t="n">
+      <c r="B8" s="31" t="n">
         <v>2239.46078431372</v>
       </c>
-      <c r="C8" s="30" t="n">
+      <c r="C8" s="32" t="n">
         <v>282150</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3715,280 +3739,280 @@
   <dimension ref="A3:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A1:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.34"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="21" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="35" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B5" s="25" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" s="36" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D5" s="26" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="37" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B6" s="27" t="n">
+        <v>386.666666666667</v>
+      </c>
+      <c r="C6" s="38" t="n">
+        <v>58000</v>
+      </c>
+      <c r="D6" s="28" t="n">
+        <v>51500</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="37" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B7" s="27" t="n">
+        <v>41.6666666666667</v>
+      </c>
+      <c r="C7" s="38" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D7" s="28" t="n">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="37" t="n">
+        <v>44351</v>
+      </c>
+      <c r="B8" s="27" t="n">
+        <v>29.1666666666667</v>
+      </c>
+      <c r="C8" s="38" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D8" s="28" t="n">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="37" t="n">
+        <v>44352</v>
+      </c>
+      <c r="B9" s="27" t="n">
+        <v>202.941176470588</v>
+      </c>
+      <c r="C9" s="38" t="n">
+        <v>34500</v>
+      </c>
+      <c r="D9" s="28" t="n">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="37" t="n">
+        <v>44353</v>
+      </c>
+      <c r="B10" s="27" t="n">
+        <v>63.3333333333333</v>
+      </c>
+      <c r="C10" s="38" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D10" s="28" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="37" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B11" s="27" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" s="38" t="n">
+        <v>7500</v>
+      </c>
+      <c r="D11" s="28" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="37" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B12" s="27" t="n">
+        <v>35.2941176470588</v>
+      </c>
+      <c r="C12" s="38" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D12" s="28" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="37" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B13" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="38" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D13" s="28" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="37" t="n">
+        <v>44357</v>
+      </c>
+      <c r="B14" s="27" t="n">
+        <v>215.294117647059</v>
+      </c>
+      <c r="C14" s="38" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D14" s="28" t="n">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="37" t="n">
+        <v>44358</v>
+      </c>
+      <c r="B15" s="27" t="n">
+        <v>64.7058823529412</v>
+      </c>
+      <c r="C15" s="38" t="n">
+        <v>11000</v>
+      </c>
+      <c r="D15" s="28" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="37" t="n">
+        <v>44359</v>
+      </c>
+      <c r="B16" s="27" t="n">
+        <v>230.392156862745</v>
+      </c>
+      <c r="C16" s="38" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D16" s="28" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="37" t="n">
+        <v>44360</v>
+      </c>
+      <c r="B17" s="27" t="n">
+        <v>8.33333333333333</v>
+      </c>
+      <c r="C17" s="38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D17" s="28" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="37" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B18" s="27" t="n">
+        <v>269.333333333333</v>
+      </c>
+      <c r="C18" s="38" t="n">
+        <v>33400</v>
+      </c>
+      <c r="D18" s="28" t="n">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="37" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B19" s="27" t="n">
+        <v>282.333333333333</v>
+      </c>
+      <c r="C19" s="38" t="n">
+        <v>42350</v>
+      </c>
+      <c r="D19" s="28" t="n">
+        <v>30400</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="37" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B20" s="29" t="n">
+        <v>250</v>
+      </c>
+      <c r="C20" s="39" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D20" s="30" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="n">
-        <v>44348</v>
-      </c>
-      <c r="B5" s="23" t="n">
-        <v>100</v>
-      </c>
-      <c r="C5" s="34" t="n">
-        <v>15000</v>
-      </c>
-      <c r="D5" s="24" t="n">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35" t="n">
-        <v>44349</v>
-      </c>
-      <c r="B6" s="25" t="n">
-        <v>386.666666666666</v>
-      </c>
-      <c r="C6" s="36" t="n">
-        <v>58000</v>
-      </c>
-      <c r="D6" s="26" t="n">
-        <v>51500</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35" t="n">
-        <v>44350</v>
-      </c>
-      <c r="B7" s="25" t="n">
-        <v>41.6666666666667</v>
-      </c>
-      <c r="C7" s="36" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D7" s="26" t="n">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="n">
-        <v>44351</v>
-      </c>
-      <c r="B8" s="25" t="n">
-        <v>29.1666666666667</v>
-      </c>
-      <c r="C8" s="36" t="n">
-        <v>3500</v>
-      </c>
-      <c r="D8" s="26" t="n">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35" t="n">
-        <v>44352</v>
-      </c>
-      <c r="B9" s="25" t="n">
-        <v>202.941176470588</v>
-      </c>
-      <c r="C9" s="36" t="n">
-        <v>34500</v>
-      </c>
-      <c r="D9" s="26" t="n">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="n">
-        <v>44353</v>
-      </c>
-      <c r="B10" s="25" t="n">
-        <v>63.3333333333333</v>
-      </c>
-      <c r="C10" s="36" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D10" s="26" t="n">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="n">
-        <v>44354</v>
-      </c>
-      <c r="B11" s="25" t="n">
-        <v>50</v>
-      </c>
-      <c r="C11" s="36" t="n">
-        <v>7500</v>
-      </c>
-      <c r="D11" s="26" t="n">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="n">
-        <v>44355</v>
-      </c>
-      <c r="B12" s="25" t="n">
-        <v>35.2941176470588</v>
-      </c>
-      <c r="C12" s="36" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D12" s="26" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="n">
-        <v>44356</v>
-      </c>
-      <c r="B13" s="25" t="n">
-        <v>10</v>
-      </c>
-      <c r="C13" s="36" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D13" s="26" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="n">
-        <v>44357</v>
-      </c>
-      <c r="B14" s="25" t="n">
-        <v>215.294117647059</v>
-      </c>
-      <c r="C14" s="36" t="n">
-        <v>35000</v>
-      </c>
-      <c r="D14" s="26" t="n">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="n">
-        <v>44358</v>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>64.7058823529412</v>
-      </c>
-      <c r="C15" s="36" t="n">
-        <v>11000</v>
-      </c>
-      <c r="D15" s="26" t="n">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="n">
-        <v>44359</v>
-      </c>
-      <c r="B16" s="25" t="n">
-        <v>230.392156862745</v>
-      </c>
-      <c r="C16" s="36" t="n">
-        <v>35000</v>
-      </c>
-      <c r="D16" s="26" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="n">
-        <v>44360</v>
-      </c>
-      <c r="B17" s="25" t="n">
-        <v>8.33333333333333</v>
-      </c>
-      <c r="C17" s="36" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D17" s="26" t="n">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="n">
-        <v>44361</v>
-      </c>
-      <c r="B18" s="25" t="n">
-        <v>269.333333333333</v>
-      </c>
-      <c r="C18" s="36" t="n">
-        <v>33400</v>
-      </c>
-      <c r="D18" s="26" t="n">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="n">
-        <v>44362</v>
-      </c>
-      <c r="B19" s="25" t="n">
-        <v>282.333333333333</v>
-      </c>
-      <c r="C19" s="36" t="n">
-        <v>42350</v>
-      </c>
-      <c r="D19" s="26" t="n">
-        <v>30400</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="n">
-        <v>44363</v>
-      </c>
-      <c r="B20" s="27" t="n">
-        <v>250</v>
-      </c>
-      <c r="C20" s="37" t="n">
-        <v>30000</v>
-      </c>
-      <c r="D20" s="28" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="29" t="n">
+      <c r="B21" s="31" t="n">
         <v>2239.46078431372</v>
       </c>
-      <c r="C21" s="39" t="n">
+      <c r="C21" s="41" t="n">
         <v>326050</v>
       </c>
-      <c r="D21" s="30" t="n">
+      <c r="D21" s="32" t="n">
         <v>282150</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
listagem de vendas realizadas
</commit_message>
<xml_diff>
--- a/application/uploads/vendas/planilha.xlsx
+++ b/application/uploads/vendas/planilha.xlsx
@@ -728,7 +728,323 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Total</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Painel_Venda_Cliente!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de Valor Faturado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472c4"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472c4"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="25560">
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Painel_Venda_Cliente!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>04819665000182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> 04055601000152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total Resultado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Painel_Venda_Cliente!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>678.872549019608</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1560.58823529412</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2239.46078431372</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1320,322 +1636,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Total</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="30"/>
-      <c:rotY val="0"/>
-      <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
-    </c:view3D>
-    <c:floor>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:backWall>
-    <c:plotArea>
-      <c:pie3DChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Painel_Venda_Cliente!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Soma de Valor Faturado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472c4"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
-              </a:solidFill>
-              <a:ln w="25560">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="a5a5a5"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Painel_Venda_Cliente!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>04819665000182</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v> 04055601000152</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total Resultado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Painel_Venda_Cliente!$B$4:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>678.872549019608</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1560.58823529412</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2239.46078431372</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-      </c:pie3DChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2360,10 +2360,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:M25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3454,29 +3454,9 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="D26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="0"/>
-      <c r="I26" s="0"/>
-      <c r="J26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="D27" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
-      <c r="J27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3496,7 +3476,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A1:M25"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3569,7 +3549,7 @@
   <dimension ref="A3:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N23" activeCellId="1" sqref="A1:M25 N23"/>
+      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3647,7 +3627,7 @@
   <dimension ref="A3:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A1:M25"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3739,7 +3719,7 @@
   <dimension ref="A3:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A1:M25"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
indicadores de vendas por servico, mensais
</commit_message>
<xml_diff>
--- a/application/uploads/vendas/planilha.xlsx
+++ b/application/uploads/vendas/planilha.xlsx
@@ -68,6 +68,72 @@
     <t xml:space="preserve">Resultado Venda</t>
   </si>
   <si>
+    <t xml:space="preserve"> 04055601000152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">becomex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaraguá do Sul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Santos Dumont,1003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88120-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste</t>
+  </si>
+  <si>
     <t xml:space="preserve">04819665000182</t>
   </si>
   <si>
@@ -80,79 +146,13 @@
     <t xml:space="preserve">Joinville</t>
   </si>
   <si>
-    <t xml:space="preserve">SC</t>
-  </si>
-  <si>
     <t xml:space="preserve">89218-060</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC</t>
-  </si>
-  <si>
     <t xml:space="preserve">FACE DIGITAL</t>
   </si>
   <si>
-    <t xml:space="preserve"> 04055601000152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">becomex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jaraguá do Sul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xyz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KTM</t>
-  </si>
-  <si>
     <t xml:space="preserve">face digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Santos Dumont,1003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88120-003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teste</t>
   </si>
   <si>
     <t xml:space="preserve">8787878000199</t>
@@ -201,11 +201,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -481,7 +482,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -523,6 +524,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,7 +733,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1044,7 +1049,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1657,8 +1662,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3418920" y="329760"/>
-        <a:ext cx="4589640" cy="2714040"/>
+        <a:off x="3418560" y="331560"/>
+        <a:ext cx="4589640" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1692,8 +1697,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4649040" y="284040"/>
-        <a:ext cx="4589280" cy="2714040"/>
+        <a:off x="4648680" y="285840"/>
+        <a:ext cx="4589640" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2360,13 +2365,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.22"/>
@@ -2444,7 +2449,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="8" t="n">
-        <v>44348</v>
+        <v>44714</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>1</v>
@@ -2454,17 +2459,17 @@
       </c>
       <c r="J2" s="9" t="n">
         <f aca="false">K2/150</f>
-        <v>100</v>
+        <v>333.333333333333</v>
       </c>
       <c r="K2" s="10" t="n">
-        <v>15000</v>
+        <v>50000</v>
       </c>
       <c r="L2" s="10" t="n">
-        <v>8000</v>
+        <v>45000</v>
       </c>
       <c r="M2" s="10" t="n">
         <f aca="false">K2-L2</f>
-        <v>7000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2480,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>16</v>
@@ -2484,10 +2489,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G3" s="8" t="n">
-        <v>44349</v>
+        <v>44696</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>1</v>
@@ -2497,17 +2502,17 @@
       </c>
       <c r="J3" s="9" t="n">
         <f aca="false">K3/150</f>
-        <v>53.3333333333333</v>
+        <v>273.333333333333</v>
       </c>
       <c r="K3" s="10" t="n">
-        <v>8000</v>
+        <v>41000</v>
       </c>
       <c r="L3" s="10" t="n">
-        <v>6500</v>
+        <v>29000</v>
       </c>
       <c r="M3" s="10" t="n">
         <f aca="false">K3-L3</f>
-        <v>1500</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2523,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>16</v>
@@ -2527,30 +2532,30 @@
         <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G4" s="8" t="n">
-        <v>44354</v>
+        <v>44361</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J4" s="9" t="n">
-        <f aca="false">K4/150</f>
-        <v>50</v>
+        <f aca="false">K4/120</f>
+        <v>233.333333333333</v>
       </c>
       <c r="K4" s="10" t="n">
-        <v>7500</v>
+        <v>28000</v>
       </c>
       <c r="L4" s="10" t="n">
-        <v>6000</v>
+        <v>27000</v>
       </c>
       <c r="M4" s="10" t="n">
         <f aca="false">K4-L4</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2558,10 +2563,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>16</v>
@@ -2570,30 +2575,30 @@
         <v>17</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G5" s="8" t="n">
-        <v>44357</v>
+        <v>44363</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J5" s="9" t="n">
-        <f aca="false">K5/150</f>
-        <v>80</v>
+        <f aca="false">K5/120</f>
+        <v>250</v>
       </c>
       <c r="K5" s="10" t="n">
-        <v>12000</v>
+        <v>30000</v>
       </c>
       <c r="L5" s="10" t="n">
-        <v>8000</v>
+        <v>30000</v>
       </c>
       <c r="M5" s="10" t="n">
         <f aca="false">K5-L5</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,7 +2609,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>16</v>
@@ -2613,30 +2618,30 @@
         <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G6" s="8" t="n">
-        <v>44361</v>
+        <v>44352</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="J6" s="9" t="n">
-        <f aca="false">K6/150</f>
-        <v>36</v>
+        <f aca="false">K6/170</f>
+        <v>188.235294117647</v>
       </c>
       <c r="K6" s="10" t="n">
-        <v>5400</v>
+        <v>32000</v>
       </c>
       <c r="L6" s="10" t="n">
-        <v>5000</v>
+        <v>30000</v>
       </c>
       <c r="M6" s="10" t="n">
         <f aca="false">K6-L6</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2647,7 +2652,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>16</v>
@@ -2656,760 +2661,760 @@
         <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>44362</v>
+        <v>44357</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="J7" s="9" t="n">
-        <f aca="false">K7/150</f>
-        <v>9</v>
+        <f aca="false">K7/170</f>
+        <v>135.294117647059</v>
       </c>
       <c r="K7" s="10" t="n">
-        <v>1350</v>
+        <v>23000</v>
       </c>
       <c r="L7" s="10" t="n">
-        <v>1400</v>
+        <v>24000</v>
       </c>
       <c r="M7" s="10" t="n">
         <f aca="false">K7-L7</f>
-        <v>-50</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G8" s="8" t="n">
-        <v>44349</v>
+        <v>44359</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="J8" s="9" t="n">
-        <f aca="false">K8/150</f>
-        <v>333.333333333333</v>
+        <f aca="false">K8/170</f>
+        <v>147.058823529412</v>
       </c>
       <c r="K8" s="10" t="n">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="L8" s="10" t="n">
-        <v>45000</v>
+        <v>22500</v>
       </c>
       <c r="M8" s="10" t="n">
         <f aca="false">K8-L8</f>
-        <v>5000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G9" s="8" t="n">
-        <v>44362</v>
+        <v>44359</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="J9" s="9" t="n">
-        <f aca="false">K9/150</f>
-        <v>273.333333333333</v>
+        <v>99</v>
       </c>
       <c r="K9" s="10" t="n">
-        <v>41000</v>
+        <v>99999</v>
       </c>
       <c r="L9" s="10" t="n">
-        <v>29000</v>
+        <v>88888</v>
       </c>
       <c r="M9" s="10" t="n">
         <f aca="false">K9-L9</f>
-        <v>12000</v>
+        <v>11111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G10" s="8" t="n">
-        <v>44350</v>
+        <v>44348</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J10" s="9" t="n">
-        <f aca="false">K10/120</f>
-        <v>41.6666666666667</v>
+        <f aca="false">K10/150</f>
+        <v>100</v>
       </c>
       <c r="K10" s="10" t="n">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="L10" s="10" t="n">
-        <v>6500</v>
+        <v>8000</v>
       </c>
       <c r="M10" s="10" t="n">
         <f aca="false">K10-L10</f>
-        <v>-1500</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G11" s="8" t="n">
-        <v>44351</v>
+        <v>44349</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J11" s="9" t="n">
-        <f aca="false">K11/120</f>
-        <v>29.1666666666667</v>
+        <f aca="false">K11/150</f>
+        <v>53.3333333333333</v>
       </c>
       <c r="K11" s="10" t="n">
-        <v>3500</v>
+        <v>8000</v>
       </c>
       <c r="L11" s="10" t="n">
-        <v>1600</v>
+        <v>6500</v>
       </c>
       <c r="M11" s="10" t="n">
         <f aca="false">K11-L11</f>
-        <v>1900</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G12" s="8" t="n">
-        <v>44353</v>
+        <v>44354</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J12" s="9" t="n">
-        <f aca="false">K12/120</f>
-        <v>63.3333333333333</v>
+        <f aca="false">K12/150</f>
+        <v>50</v>
       </c>
       <c r="K12" s="10" t="n">
-        <v>7600</v>
+        <v>7500</v>
       </c>
       <c r="L12" s="10" t="n">
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="M12" s="10" t="n">
         <f aca="false">K12-L12</f>
-        <v>600</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G13" s="8" t="n">
-        <v>44356</v>
+        <v>44357</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J13" s="9" t="n">
-        <f aca="false">K13/120</f>
-        <v>10</v>
+        <f aca="false">K13/150</f>
+        <v>80</v>
       </c>
       <c r="K13" s="10" t="n">
-        <v>1200</v>
+        <v>12000</v>
       </c>
       <c r="L13" s="10" t="n">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="M13" s="10" t="n">
         <f aca="false">K13-L13</f>
-        <v>-3800</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G14" s="8" t="n">
-        <v>44359</v>
+        <v>44361</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J14" s="9" t="n">
-        <f aca="false">K14/120</f>
-        <v>83.3333333333333</v>
+        <f aca="false">K14/150</f>
+        <v>36</v>
       </c>
       <c r="K14" s="10" t="n">
-        <v>10000</v>
+        <v>5400</v>
       </c>
       <c r="L14" s="10" t="n">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="M14" s="10" t="n">
         <f aca="false">K14-L14</f>
-        <v>2500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G15" s="8" t="n">
-        <v>44360</v>
+        <v>44362</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J15" s="9" t="n">
-        <f aca="false">K15/120</f>
-        <v>8.33333333333333</v>
+        <f aca="false">K15/150</f>
+        <v>9</v>
       </c>
       <c r="K15" s="10" t="n">
-        <v>1000</v>
+        <v>1350</v>
       </c>
       <c r="L15" s="10" t="n">
-        <v>650</v>
+        <v>1400</v>
       </c>
       <c r="M15" s="10" t="n">
         <f aca="false">K15-L15</f>
-        <v>350</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G16" s="8" t="n">
-        <v>44361</v>
+        <v>44350</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J16" s="9" t="n">
         <f aca="false">K16/120</f>
-        <v>233.333333333333</v>
+        <v>41.6666666666667</v>
       </c>
       <c r="K16" s="10" t="n">
-        <v>28000</v>
+        <v>5000</v>
       </c>
       <c r="L16" s="10" t="n">
-        <v>27000</v>
+        <v>6500</v>
       </c>
       <c r="M16" s="10" t="n">
         <f aca="false">K16-L16</f>
-        <v>1000</v>
+        <v>-1500</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>44363</v>
+        <v>44351</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J17" s="9" t="n">
         <f aca="false">K17/120</f>
-        <v>250</v>
+        <v>29.1666666666667</v>
       </c>
       <c r="K17" s="10" t="n">
-        <v>30000</v>
+        <v>3500</v>
       </c>
       <c r="L17" s="10" t="n">
-        <v>30000</v>
+        <v>1600</v>
       </c>
       <c r="M17" s="10" t="n">
         <f aca="false">K17-L17</f>
-        <v>0</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G18" s="8" t="n">
-        <v>44352</v>
+        <v>44353</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J18" s="9" t="n">
-        <f aca="false">K18/170</f>
-        <v>14.7058823529412</v>
+        <f aca="false">K18/120</f>
+        <v>63.3333333333333</v>
       </c>
       <c r="K18" s="10" t="n">
-        <v>2500</v>
+        <v>7600</v>
       </c>
       <c r="L18" s="10" t="n">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="M18" s="10" t="n">
         <f aca="false">K18-L18</f>
-        <v>-500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G19" s="8" t="n">
-        <v>44355</v>
+        <v>44356</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J19" s="9" t="n">
-        <f aca="false">K19/170</f>
-        <v>35.2941176470588</v>
+        <f aca="false">K19/120</f>
+        <v>10</v>
       </c>
       <c r="K19" s="10" t="n">
-        <v>6000</v>
+        <v>1200</v>
       </c>
       <c r="L19" s="10" t="n">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="M19" s="10" t="n">
         <f aca="false">K19-L19</f>
-        <v>5500</v>
+        <v>-3800</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G20" s="8" t="n">
-        <v>44358</v>
+        <v>44359</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J20" s="9" t="n">
-        <f aca="false">K20/170</f>
-        <v>64.7058823529412</v>
+        <f aca="false">K20/120</f>
+        <v>83.3333333333333</v>
       </c>
       <c r="K20" s="10" t="n">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="L20" s="10" t="n">
-        <v>8000</v>
+        <v>7500</v>
       </c>
       <c r="M20" s="10" t="n">
         <f aca="false">K20-L20</f>
-        <v>3000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G21" s="8" t="n">
-        <v>44352</v>
+        <v>44360</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J21" s="9" t="n">
-        <f aca="false">K21/170</f>
-        <v>188.235294117647</v>
+        <f aca="false">K21/120</f>
+        <v>8.33333333333333</v>
       </c>
       <c r="K21" s="10" t="n">
-        <v>32000</v>
+        <v>1000</v>
       </c>
       <c r="L21" s="10" t="n">
-        <v>30000</v>
+        <v>650</v>
       </c>
       <c r="M21" s="10" t="n">
         <f aca="false">K21-L21</f>
-        <v>2000</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G22" s="8" t="n">
-        <v>44357</v>
+        <v>44352</v>
       </c>
       <c r="H22" s="2" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J22" s="9" t="n">
         <f aca="false">K22/170</f>
-        <v>135.294117647059</v>
+        <v>14.7058823529412</v>
       </c>
       <c r="K22" s="10" t="n">
-        <v>23000</v>
+        <v>2500</v>
       </c>
       <c r="L22" s="10" t="n">
-        <v>24000</v>
+        <v>3000</v>
       </c>
       <c r="M22" s="10" t="n">
         <f aca="false">K22-L22</f>
-        <v>-1000</v>
+        <v>-500</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G23" s="8" t="n">
-        <v>44359</v>
+        <v>44355</v>
       </c>
       <c r="H23" s="2" t="n">
         <v>3</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J23" s="9" t="n">
         <f aca="false">K23/170</f>
-        <v>147.058823529412</v>
+        <v>35.2941176470588</v>
       </c>
       <c r="K23" s="10" t="n">
-        <v>25000</v>
+        <v>6000</v>
       </c>
       <c r="L23" s="10" t="n">
-        <v>22500</v>
+        <v>500</v>
       </c>
       <c r="M23" s="10" t="n">
         <f aca="false">K23-L23</f>
-        <v>2500</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G24" s="8" t="n">
-        <v>44359</v>
+        <v>44358</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J24" s="9" t="n">
-        <v>99</v>
+        <f aca="false">K24/170</f>
+        <v>64.7058823529412</v>
       </c>
       <c r="K24" s="10" t="n">
-        <v>99999</v>
+        <v>11000</v>
       </c>
       <c r="L24" s="10" t="n">
-        <v>88888</v>
+        <v>8000</v>
       </c>
       <c r="M24" s="10" t="n">
         <f aca="false">K24-L24</f>
-        <v>11111</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3422,7 @@
         <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>43</v>
@@ -3454,12 +3459,24 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="11"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3479,14 +3496,14 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.78"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>47</v>
       </c>
@@ -3497,7 +3514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
@@ -3508,7 +3525,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
@@ -3519,12 +3536,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>170</v>
@@ -3532,7 +3549,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3552,45 +3569,45 @@
       <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="15" t="n">
+        <v>678.872549019608</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="14" t="n">
-        <v>678.872549019608</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="16" t="n">
+      <c r="B5" s="17" t="n">
         <v>1560.58823529412</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="19" t="n">
         <v>2239.46078431372</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="0" t="n">
         <v>1837</v>
       </c>
@@ -3598,7 +3615,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L24" s="0" t="n">
         <v>1080</v>
       </c>
@@ -3609,7 +3626,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3630,78 +3647,78 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.34"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20" t="s">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="25" t="n">
+      <c r="B5" s="26" t="n">
         <v>935</v>
       </c>
-      <c r="C5" s="26" t="n">
+      <c r="C5" s="27" t="n">
         <v>108900</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="27" t="n">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="28" t="n">
         <v>585.294117647059</v>
       </c>
-      <c r="C6" s="28" t="n">
+      <c r="C6" s="29" t="n">
         <v>88000</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="29" t="n">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="30" t="n">
         <v>719.166666666667</v>
       </c>
-      <c r="C7" s="30" t="n">
+      <c r="C7" s="31" t="n">
         <v>85250</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="31" t="n">
+      <c r="B8" s="32" t="n">
         <v>2239.46078431372</v>
       </c>
-      <c r="C8" s="32" t="n">
+      <c r="C8" s="33" t="n">
         <v>282150</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3722,7 +3739,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
@@ -3730,269 +3747,269 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.34"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20" t="s">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35" t="n">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="36" t="n">
         <v>44348</v>
       </c>
-      <c r="B5" s="25" t="n">
+      <c r="B5" s="26" t="n">
         <v>100</v>
       </c>
-      <c r="C5" s="36" t="n">
+      <c r="C5" s="37" t="n">
         <v>15000</v>
       </c>
-      <c r="D5" s="26" t="n">
+      <c r="D5" s="27" t="n">
         <v>8000</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="n">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="38" t="n">
         <v>44349</v>
       </c>
-      <c r="B6" s="27" t="n">
+      <c r="B6" s="28" t="n">
         <v>386.666666666667</v>
       </c>
-      <c r="C6" s="38" t="n">
+      <c r="C6" s="39" t="n">
         <v>58000</v>
       </c>
-      <c r="D6" s="28" t="n">
+      <c r="D6" s="29" t="n">
         <v>51500</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="n">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="38" t="n">
         <v>44350</v>
       </c>
-      <c r="B7" s="27" t="n">
+      <c r="B7" s="28" t="n">
         <v>41.6666666666667</v>
       </c>
-      <c r="C7" s="38" t="n">
+      <c r="C7" s="39" t="n">
         <v>5000</v>
       </c>
-      <c r="D7" s="28" t="n">
+      <c r="D7" s="29" t="n">
         <v>6500</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="n">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="38" t="n">
         <v>44351</v>
       </c>
-      <c r="B8" s="27" t="n">
+      <c r="B8" s="28" t="n">
         <v>29.1666666666667</v>
       </c>
-      <c r="C8" s="38" t="n">
+      <c r="C8" s="39" t="n">
         <v>3500</v>
       </c>
-      <c r="D8" s="28" t="n">
+      <c r="D8" s="29" t="n">
         <v>1600</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="n">
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="38" t="n">
         <v>44352</v>
       </c>
-      <c r="B9" s="27" t="n">
+      <c r="B9" s="28" t="n">
         <v>202.941176470588</v>
       </c>
-      <c r="C9" s="38" t="n">
+      <c r="C9" s="39" t="n">
         <v>34500</v>
       </c>
-      <c r="D9" s="28" t="n">
+      <c r="D9" s="29" t="n">
         <v>33000</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="n">
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="38" t="n">
         <v>44353</v>
       </c>
-      <c r="B10" s="27" t="n">
+      <c r="B10" s="28" t="n">
         <v>63.3333333333333</v>
       </c>
-      <c r="C10" s="38" t="n">
+      <c r="C10" s="39" t="n">
         <v>7600</v>
       </c>
-      <c r="D10" s="28" t="n">
+      <c r="D10" s="29" t="n">
         <v>7000</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="n">
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="38" t="n">
         <v>44354</v>
       </c>
-      <c r="B11" s="27" t="n">
+      <c r="B11" s="28" t="n">
         <v>50</v>
       </c>
-      <c r="C11" s="38" t="n">
+      <c r="C11" s="39" t="n">
         <v>7500</v>
       </c>
-      <c r="D11" s="28" t="n">
+      <c r="D11" s="29" t="n">
         <v>6000</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="n">
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="38" t="n">
         <v>44355</v>
       </c>
-      <c r="B12" s="27" t="n">
+      <c r="B12" s="28" t="n">
         <v>35.2941176470588</v>
       </c>
-      <c r="C12" s="38" t="n">
+      <c r="C12" s="39" t="n">
         <v>6000</v>
       </c>
-      <c r="D12" s="28" t="n">
+      <c r="D12" s="29" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="n">
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="n">
         <v>44356</v>
       </c>
-      <c r="B13" s="27" t="n">
+      <c r="B13" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="C13" s="38" t="n">
+      <c r="C13" s="39" t="n">
         <v>1200</v>
       </c>
-      <c r="D13" s="28" t="n">
+      <c r="D13" s="29" t="n">
         <v>5000</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="n">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="n">
         <v>44357</v>
       </c>
-      <c r="B14" s="27" t="n">
+      <c r="B14" s="28" t="n">
         <v>215.294117647059</v>
       </c>
-      <c r="C14" s="38" t="n">
+      <c r="C14" s="39" t="n">
         <v>35000</v>
       </c>
-      <c r="D14" s="28" t="n">
+      <c r="D14" s="29" t="n">
         <v>32000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="n">
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="38" t="n">
         <v>44358</v>
       </c>
-      <c r="B15" s="27" t="n">
+      <c r="B15" s="28" t="n">
         <v>64.7058823529412</v>
       </c>
-      <c r="C15" s="38" t="n">
+      <c r="C15" s="39" t="n">
         <v>11000</v>
       </c>
-      <c r="D15" s="28" t="n">
+      <c r="D15" s="29" t="n">
         <v>8000</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="n">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="38" t="n">
         <v>44359</v>
       </c>
-      <c r="B16" s="27" t="n">
+      <c r="B16" s="28" t="n">
         <v>230.392156862745</v>
       </c>
-      <c r="C16" s="38" t="n">
+      <c r="C16" s="39" t="n">
         <v>35000</v>
       </c>
-      <c r="D16" s="28" t="n">
+      <c r="D16" s="29" t="n">
         <v>30000</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="n">
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="38" t="n">
         <v>44360</v>
       </c>
-      <c r="B17" s="27" t="n">
+      <c r="B17" s="28" t="n">
         <v>8.33333333333333</v>
       </c>
-      <c r="C17" s="38" t="n">
+      <c r="C17" s="39" t="n">
         <v>1000</v>
       </c>
-      <c r="D17" s="28" t="n">
+      <c r="D17" s="29" t="n">
         <v>650</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="n">
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="38" t="n">
         <v>44361</v>
       </c>
-      <c r="B18" s="27" t="n">
+      <c r="B18" s="28" t="n">
         <v>269.333333333333</v>
       </c>
-      <c r="C18" s="38" t="n">
+      <c r="C18" s="39" t="n">
         <v>33400</v>
       </c>
-      <c r="D18" s="28" t="n">
+      <c r="D18" s="29" t="n">
         <v>32000</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="n">
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="38" t="n">
         <v>44362</v>
       </c>
-      <c r="B19" s="27" t="n">
+      <c r="B19" s="28" t="n">
         <v>282.333333333333</v>
       </c>
-      <c r="C19" s="38" t="n">
+      <c r="C19" s="39" t="n">
         <v>42350</v>
       </c>
-      <c r="D19" s="28" t="n">
+      <c r="D19" s="29" t="n">
         <v>30400</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="n">
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="38" t="n">
         <v>44363</v>
       </c>
-      <c r="B20" s="29" t="n">
+      <c r="B20" s="30" t="n">
         <v>250</v>
       </c>
-      <c r="C20" s="39" t="n">
+      <c r="C20" s="40" t="n">
         <v>30000</v>
       </c>
-      <c r="D20" s="30" t="n">
+      <c r="D20" s="31" t="n">
         <v>30000</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40" t="s">
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="31" t="n">
+      <c r="B21" s="32" t="n">
         <v>2239.46078431372</v>
       </c>
-      <c r="C21" s="41" t="n">
+      <c r="C21" s="42" t="n">
         <v>326050</v>
       </c>
-      <c r="D21" s="32" t="n">
+      <c r="D21" s="33" t="n">
         <v>282150</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>